<commit_message>
Se actualizaron mas lentes
Nuevos lentes sigma se subieron a la Base
</commit_message>
<xml_diff>
--- a/productos_sony_lentes_maestra.xlsx
+++ b/productos_sony_lentes_maestra.xlsx
@@ -25,7 +25,7 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="63" r:id="rId4"/>
+    <pivotCache cacheId="91" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1012" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1102" uniqueCount="270">
   <si>
     <t>Producto</t>
   </si>
@@ -815,6 +815,45 @@
   </si>
   <si>
     <t>Zeiss Batis 85mm F/1,8 FE</t>
+  </si>
+  <si>
+    <t>Sigma 45mm F/2,8 FE</t>
+  </si>
+  <si>
+    <t>Sigma 65mm f/2 DG DN Contemporary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sigma 60mm F/2,8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sigma 19mm F/2,8 </t>
+  </si>
+  <si>
+    <t>Fotos de Calle, Paisajes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sigma 30mm F/2,8 </t>
+  </si>
+  <si>
+    <t>Fotos de Calle</t>
+  </si>
+  <si>
+    <t>SIGMA 90mm F/2,8 DG DN Contemporary</t>
+  </si>
+  <si>
+    <t>Viltrox AF 13mm f/1.4 E, para Sony E</t>
+  </si>
+  <si>
+    <t>Yongnuo YN56mm F1.4S DA DSM para Sony E</t>
+  </si>
+  <si>
+    <t>Yongnuo YN33mm F1.4S DA DSM para Sony E</t>
+  </si>
+  <si>
+    <t>FE 16-35mm F2.8 | GMASTER</t>
+  </si>
+  <si>
+    <t>FE 70-200 mm F4 Macro G OSS II</t>
   </si>
 </sst>
 </file>
@@ -1096,7 +1135,7 @@
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1154,12 +1193,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="6" fillId="4" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1193,6 +1226,15 @@
     <xf numFmtId="44" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
@@ -1200,16 +1242,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="16">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1675,6 +1707,16 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1994,7 +2036,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Ortega Mazzini, David" refreshedDate="45653.492214004633" createdVersion="8" refreshedVersion="6" minRefreshableVersion="3" recordCount="142">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Ortega Mazzini, David" refreshedDate="45656.618045370371" createdVersion="8" refreshedVersion="6" minRefreshableVersion="3" recordCount="151">
   <cacheSource type="worksheet">
     <worksheetSource name="Datos"/>
   </cacheSource>
@@ -2036,12 +2078,12 @@
         <s v="Teleobjetivo y SuperTeleobjetivo"/>
         <s v="Gran Angular - Angular"/>
         <s v="Angular - Teleobjetivo"/>
-        <m/>
         <s v="Angular Teleobjetivo"/>
         <s v="Telecorto -  Teleobjetivo"/>
         <s v="Teleobjetivo - Super Tele"/>
         <s v="Angular Tele corto"/>
         <s v="Ultra Gran Angular"/>
+        <m u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Uso" numFmtId="0">
@@ -2054,7 +2096,7 @@
       </sharedItems>
     </cacheField>
     <cacheField name="Nombre" numFmtId="0">
-      <sharedItems count="147">
+      <sharedItems count="158">
         <s v="FE 85 mm F1.4 GM II"/>
         <s v="Lente E PZ 16-50 mm F3.5-5.6 OSS II"/>
         <s v="FE 16-25 mm F2.8 G"/>
@@ -2197,11 +2239,22 @@
         <s v="Zeiss Batis 18mm F/2,8 FE"/>
         <s v="Zeiss Batis 135mm F/2,8 FE"/>
         <s v="Zeiss Batis 85mm F/1,8 FE"/>
+        <s v="Sigma 45mm F/2,8 FE"/>
+        <s v="Sigma 65mm f/2 DG DN Contemporary"/>
+        <s v="Sigma 60mm F/2,8 "/>
+        <s v="Sigma 19mm F/2,8 "/>
+        <s v="Sigma 30mm F/2,8 "/>
+        <s v="SIGMA 90mm F/2,8 DG DN Contemporary"/>
+        <s v="Viltrox AF 13mm f/1.4 E, para Sony E"/>
+        <s v="Yongnuo YN33mm F1.4S DA DSM para Sony E"/>
+        <s v="Yongnuo YN56mm F1.4S DA DSM para Sony E"/>
         <s v="Viltrox 75mm f/1.2 AF, APS-C para Sony E" u="1"/>
         <s v="Viltrox AF 75mm f/1.2, APS-C para Sony E" u="1"/>
         <s v="Viltrox AF 28mm f/1,8 FE, Full Frame, para Sony" u="1"/>
         <s v="Viltrox AF 28mm f/1.8 FE, Full Frame, para Sony" u="1"/>
+        <s v="Tamron AF 11-20mm f/2.8 Di III VXD para Sony E" u="1"/>
         <s v="Samyanf AF 24mm F/2,8 FE" u="1"/>
+        <s v="Sigma 24mm f/1.4 DG DN Art" u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Precio" numFmtId="44">
@@ -2229,7 +2282,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="142">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="151">
   <r>
     <x v="0"/>
     <x v="0"/>
@@ -3312,7 +3365,7 @@
   <r>
     <x v="0"/>
     <x v="5"/>
-    <x v="14"/>
+    <x v="5"/>
     <m/>
     <x v="0"/>
     <x v="83"/>
@@ -3507,7 +3560,7 @@
   <r>
     <x v="1"/>
     <x v="1"/>
-    <x v="15"/>
+    <x v="14"/>
     <s v="Viajes, Bodas, Retratos, Foto de Producto"/>
     <x v="1"/>
     <x v="98"/>
@@ -3520,7 +3573,7 @@
   <r>
     <x v="1"/>
     <x v="1"/>
-    <x v="15"/>
+    <x v="14"/>
     <s v="Viajes, Bodas, Retratos, Foto de Producto"/>
     <x v="1"/>
     <x v="99"/>
@@ -3585,7 +3638,7 @@
   <r>
     <x v="1"/>
     <x v="1"/>
-    <x v="15"/>
+    <x v="14"/>
     <s v="Viajes, Bodas, Retratos, Foto de Producto"/>
     <x v="0"/>
     <x v="104"/>
@@ -3637,7 +3690,7 @@
   <r>
     <x v="1"/>
     <x v="1"/>
-    <x v="16"/>
+    <x v="15"/>
     <s v="Retratos, Bodas, Deportes, Vida Silvestre"/>
     <x v="0"/>
     <x v="108"/>
@@ -3741,7 +3794,7 @@
   <r>
     <x v="1"/>
     <x v="1"/>
-    <x v="17"/>
+    <x v="16"/>
     <s v="Vida Salvaje"/>
     <x v="0"/>
     <x v="116"/>
@@ -3754,7 +3807,7 @@
   <r>
     <x v="1"/>
     <x v="1"/>
-    <x v="17"/>
+    <x v="16"/>
     <s v="Vida Salvaje"/>
     <x v="0"/>
     <x v="117"/>
@@ -3767,7 +3820,7 @@
   <r>
     <x v="1"/>
     <x v="1"/>
-    <x v="18"/>
+    <x v="17"/>
     <s v="Vlog"/>
     <x v="0"/>
     <x v="118"/>
@@ -3923,7 +3976,7 @@
   <r>
     <x v="1"/>
     <x v="7"/>
-    <x v="16"/>
+    <x v="15"/>
     <s v="Retratos, Bodas, Foto de Producto, Viajes"/>
     <x v="0"/>
     <x v="130"/>
@@ -4001,7 +4054,7 @@
   <r>
     <x v="0"/>
     <x v="8"/>
-    <x v="19"/>
+    <x v="18"/>
     <s v="Paisajes, Arquitectura, Bienes Raices"/>
     <x v="0"/>
     <x v="136"/>
@@ -4071,6 +4124,123 @@
     <x v="0"/>
     <x v="141"/>
     <n v="1199"/>
+    <n v="4"/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <s v="Vlog, Paisajes, Videos Youtube"/>
+    <x v="0"/>
+    <x v="142"/>
+    <n v="445"/>
+    <n v="4"/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="0"/>
+    <s v="Retratos, Foto de Producto"/>
+    <x v="0"/>
+    <x v="143"/>
+    <n v="699"/>
+    <n v="4"/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="0"/>
+    <s v="Retratos, Foto de Producto"/>
+    <x v="1"/>
+    <x v="144"/>
+    <n v="180"/>
+    <n v="5"/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="8"/>
+    <s v="Fotos de Calle, Paisajes"/>
+    <x v="1"/>
+    <x v="145"/>
+    <n v="180"/>
+    <n v="3.5"/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="8"/>
+    <s v="Fotos de Calle"/>
+    <x v="1"/>
+    <x v="146"/>
+    <n v="180"/>
+    <n v="3.5"/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="0"/>
+    <s v="Retratos"/>
+    <x v="0"/>
+    <x v="147"/>
+    <n v="699"/>
+    <n v="5"/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="2"/>
+    <s v="Vlog, Paisajes, Videos Youtube"/>
+    <x v="1"/>
+    <x v="148"/>
+    <n v="413"/>
+    <n v="4"/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="4"/>
+    <x v="0"/>
+    <s v="Foto de Calle, Retratos"/>
+    <x v="1"/>
+    <x v="149"/>
+    <n v="320"/>
+    <n v="4"/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="4"/>
+    <x v="0"/>
+    <s v="Foto de Calle, Retratos"/>
+    <x v="1"/>
+    <x v="150"/>
+    <n v="345"/>
     <n v="4"/>
     <m/>
     <m/>
@@ -4080,8 +4250,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica1" cacheId="63" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Producto">
-  <location ref="A3:B12" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica1" cacheId="91" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Producto">
+  <location ref="A3:B48" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField showAll="0">
       <items count="4">
@@ -4096,9 +4266,9 @@
         <item h="1" x="8"/>
         <item h="1" x="7"/>
         <item h="1" x="2"/>
-        <item h="1" x="0"/>
+        <item x="0"/>
         <item h="1" x="1"/>
-        <item x="5"/>
+        <item h="1" x="5"/>
         <item h="1" x="6"/>
         <item h="1" x="3"/>
         <item h="1" x="4"/>
@@ -4109,9 +4279,9 @@
       <items count="21">
         <item x="8"/>
         <item x="13"/>
-        <item x="18"/>
+        <item x="17"/>
         <item x="3"/>
-        <item x="15"/>
+        <item x="14"/>
         <item x="10"/>
         <item x="2"/>
         <item x="12"/>
@@ -4119,27 +4289,27 @@
         <item x="9"/>
         <item x="4"/>
         <item x="0"/>
+        <item x="15"/>
+        <item x="5"/>
         <item x="16"/>
-        <item x="5"/>
-        <item x="17"/>
         <item x="11"/>
         <item x="7"/>
-        <item x="19"/>
+        <item x="18"/>
         <item x="6"/>
-        <item x="14"/>
+        <item m="1" x="19"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField showAll="0"/>
     <pivotField showAll="0">
       <items count="3">
-        <item x="1"/>
+        <item h="1" x="1"/>
         <item x="0"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField axis="axisRow" showAll="0" sortType="ascending">
-      <items count="148">
+      <items count="159">
         <item x="60"/>
         <item x="20"/>
         <item x="19"/>
@@ -4198,7 +4368,7 @@
         <item x="5"/>
         <item x="49"/>
         <item x="61"/>
-        <item m="1" x="146"/>
+        <item m="1" x="156"/>
         <item x="133"/>
         <item x="132"/>
         <item x="129"/>
@@ -4215,14 +4385,21 @@
         <item x="64"/>
         <item x="82"/>
         <item x="93"/>
+        <item x="145"/>
         <item x="68"/>
+        <item m="1" x="157"/>
         <item x="92"/>
         <item x="94"/>
+        <item x="146"/>
         <item x="81"/>
         <item x="105"/>
         <item x="80"/>
+        <item x="142"/>
         <item x="122"/>
         <item x="91"/>
+        <item x="144"/>
+        <item x="143"/>
+        <item x="147"/>
         <item x="40"/>
         <item x="36"/>
         <item x="109"/>
@@ -4240,6 +4417,7 @@
         <item x="101"/>
         <item x="62"/>
         <item x="102"/>
+        <item m="1" x="155"/>
         <item x="116"/>
         <item x="99"/>
         <item x="118"/>
@@ -4259,14 +4437,15 @@
         <item x="58"/>
         <item x="41"/>
         <item x="43"/>
-        <item m="1" x="142"/>
+        <item m="1" x="151"/>
+        <item x="148"/>
         <item x="121"/>
         <item x="72"/>
         <item x="74"/>
         <item x="75"/>
         <item x="71"/>
-        <item m="1" x="144"/>
-        <item m="1" x="145"/>
+        <item m="1" x="153"/>
+        <item m="1" x="154"/>
         <item x="124"/>
         <item x="66"/>
         <item x="77"/>
@@ -4275,13 +4454,15 @@
         <item x="76"/>
         <item x="78"/>
         <item x="119"/>
-        <item m="1" x="143"/>
+        <item m="1" x="152"/>
         <item x="120"/>
         <item x="69"/>
         <item x="113"/>
+        <item x="149"/>
         <item x="95"/>
         <item x="97"/>
         <item x="89"/>
+        <item x="150"/>
         <item x="87"/>
         <item x="140"/>
         <item x="139"/>
@@ -4299,30 +4480,138 @@
   <rowFields count="1">
     <field x="5"/>
   </rowFields>
-  <rowItems count="9">
+  <rowItems count="45">
     <i>
-      <x v="104"/>
+      <x v="14"/>
     </i>
     <i>
-      <x v="105"/>
+      <x v="15"/>
     </i>
     <i>
-      <x v="106"/>
+      <x v="16"/>
     </i>
     <i>
-      <x v="107"/>
+      <x v="17"/>
     </i>
     <i>
-      <x v="108"/>
+      <x v="18"/>
     </i>
     <i>
-      <x v="109"/>
+      <x v="19"/>
     </i>
     <i>
-      <x v="110"/>
+      <x v="20"/>
     </i>
     <i>
-      <x v="111"/>
+      <x v="21"/>
+    </i>
+    <i>
+      <x v="22"/>
+    </i>
+    <i>
+      <x v="23"/>
+    </i>
+    <i>
+      <x v="24"/>
+    </i>
+    <i>
+      <x v="25"/>
+    </i>
+    <i>
+      <x v="26"/>
+    </i>
+    <i>
+      <x v="27"/>
+    </i>
+    <i>
+      <x v="28"/>
+    </i>
+    <i>
+      <x v="29"/>
+    </i>
+    <i>
+      <x v="30"/>
+    </i>
+    <i>
+      <x v="31"/>
+    </i>
+    <i>
+      <x v="32"/>
+    </i>
+    <i>
+      <x v="33"/>
+    </i>
+    <i>
+      <x v="34"/>
+    </i>
+    <i>
+      <x v="35"/>
+    </i>
+    <i>
+      <x v="36"/>
+    </i>
+    <i>
+      <x v="37"/>
+    </i>
+    <i>
+      <x v="38"/>
+    </i>
+    <i>
+      <x v="39"/>
+    </i>
+    <i>
+      <x v="40"/>
+    </i>
+    <i>
+      <x v="41"/>
+    </i>
+    <i>
+      <x v="42"/>
+    </i>
+    <i>
+      <x v="43"/>
+    </i>
+    <i>
+      <x v="44"/>
+    </i>
+    <i>
+      <x v="45"/>
+    </i>
+    <i>
+      <x v="46"/>
+    </i>
+    <i>
+      <x v="47"/>
+    </i>
+    <i>
+      <x v="48"/>
+    </i>
+    <i>
+      <x v="49"/>
+    </i>
+    <i>
+      <x v="52"/>
+    </i>
+    <i>
+      <x v="53"/>
+    </i>
+    <i>
+      <x v="54"/>
+    </i>
+    <i>
+      <x v="55"/>
+    </i>
+    <i>
+      <x v="57"/>
+    </i>
+    <i>
+      <x v="91"/>
+    </i>
+    <i>
+      <x v="125"/>
+    </i>
+    <i>
+      <x v="126"/>
     </i>
     <i t="grand">
       <x/>
@@ -4354,9 +4643,9 @@
   <data>
     <tabular pivotCacheId="952029092">
       <items count="3">
+        <i x="2" s="1"/>
         <i x="0" s="1"/>
         <i x="1" s="1"/>
-        <i x="2" s="1" nd="1"/>
       </items>
     </tabular>
   </data>
@@ -4372,25 +4661,25 @@
     <tabular pivotCacheId="952029092">
       <items count="20">
         <i x="8" s="1"/>
+        <i x="3" s="1"/>
+        <i x="10" s="1"/>
+        <i x="2" s="1"/>
+        <i x="1" s="1"/>
         <i x="9" s="1"/>
+        <i x="4" s="1"/>
         <i x="0" s="1"/>
-        <i x="14" s="1"/>
+        <i x="5" s="1"/>
+        <i x="7" s="1"/>
         <i x="13" s="1" nd="1"/>
+        <i x="17" s="1" nd="1"/>
+        <i x="14" s="1" nd="1"/>
+        <i x="12" s="1" nd="1"/>
+        <i x="15" s="1" nd="1"/>
+        <i x="16" s="1" nd="1"/>
+        <i x="11" s="1" nd="1"/>
         <i x="18" s="1" nd="1"/>
-        <i x="3" s="1" nd="1"/>
-        <i x="15" s="1" nd="1"/>
-        <i x="10" s="1" nd="1"/>
-        <i x="2" s="1" nd="1"/>
-        <i x="12" s="1" nd="1"/>
-        <i x="1" s="1" nd="1"/>
-        <i x="4" s="1" nd="1"/>
-        <i x="16" s="1" nd="1"/>
-        <i x="5" s="1" nd="1"/>
-        <i x="17" s="1" nd="1"/>
-        <i x="11" s="1" nd="1"/>
-        <i x="7" s="1" nd="1"/>
+        <i x="6" s="1" nd="1"/>
         <i x="19" s="1" nd="1"/>
-        <i x="6" s="1" nd="1"/>
       </items>
     </tabular>
   </data>
@@ -4408,9 +4697,9 @@
         <i x="8"/>
         <i x="7"/>
         <i x="2"/>
-        <i x="0"/>
+        <i x="0" s="1"/>
         <i x="1"/>
-        <i x="5" s="1"/>
+        <i x="5"/>
         <i x="6"/>
         <i x="3"/>
         <i x="4"/>
@@ -4429,7 +4718,7 @@
   <data>
     <tabular pivotCacheId="952029092">
       <items count="2">
-        <i x="1" s="1"/>
+        <i x="1"/>
         <i x="0" s="1"/>
       </items>
     </tabular>
@@ -4441,26 +4730,26 @@
 <slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
   <slicer name="Tipo" cache="SegmentaciónDeDatos_Tipo" caption="Tipo" style="SlicerStyleLight2" rowHeight="241300"/>
   <slicer name="Categoria" cache="SegmentaciónDeDatos_Categoria" caption="Categoria" style="SlicerStyleDark4" rowHeight="241300"/>
-  <slicer name="Marca" cache="SegmentaciónDeDatos_Marca" caption="Marca" rowHeight="241300"/>
+  <slicer name="Marca" cache="SegmentaciónDeDatos_Marca" caption="Marca" startItem="2" rowHeight="241300"/>
   <slicer name="Sensor" cache="SegmentaciónDeDatos_Sensor" caption="Sensor" style="SlicerStyleDark6" rowHeight="241300"/>
 </slicers>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Datos" displayName="Datos" ref="A1:K143" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12">
-  <autoFilter ref="A1:K143"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Datos" displayName="Datos" ref="A1:K152" totalsRowShown="0" headerRowDxfId="14" dataDxfId="12" headerRowBorderDxfId="13" tableBorderDxfId="11">
+  <autoFilter ref="A1:K152"/>
   <tableColumns count="11">
-    <tableColumn id="1" name="Tipo" dataDxfId="11"/>
-    <tableColumn id="9" name="Marca" dataDxfId="10"/>
-    <tableColumn id="2" name="Categoria" dataDxfId="9"/>
-    <tableColumn id="3" name="Uso" dataDxfId="8"/>
-    <tableColumn id="4" name="Sensor" dataDxfId="7"/>
-    <tableColumn id="5" name="Nombre" dataDxfId="6"/>
-    <tableColumn id="6" name="Precio" dataDxfId="5" dataCellStyle="Moneda"/>
-    <tableColumn id="7" name="Calificacion" dataDxfId="4"/>
-    <tableColumn id="8" name="Tamaño de Filtro" dataDxfId="3"/>
-    <tableColumn id="10" name="Distancia Minima de Enfoque" dataDxfId="2"/>
-    <tableColumn id="11" name="Peso" dataDxfId="1"/>
+    <tableColumn id="1" name="Tipo" dataDxfId="10"/>
+    <tableColumn id="9" name="Marca" dataDxfId="9"/>
+    <tableColumn id="2" name="Categoria" dataDxfId="8"/>
+    <tableColumn id="3" name="Uso" dataDxfId="7"/>
+    <tableColumn id="4" name="Sensor" dataDxfId="6"/>
+    <tableColumn id="5" name="Nombre" dataDxfId="5"/>
+    <tableColumn id="6" name="Precio" dataDxfId="4" dataCellStyle="Moneda"/>
+    <tableColumn id="7" name="Calificacion" dataDxfId="3"/>
+    <tableColumn id="8" name="Tamaño de Filtro" dataDxfId="2"/>
+    <tableColumn id="10" name="Distancia Minima de Enfoque" dataDxfId="1"/>
+    <tableColumn id="11" name="Peso" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4768,14 +5057,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="48" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="D1" s="30" t="s">
+      <c r="B1" s="48"/>
+      <c r="D1" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="E1" s="30"/>
+      <c r="E1" s="49"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -5916,7 +6205,7 @@
     <mergeCell ref="D1:E1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G64">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
       <formula>"Mismo Precio"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5927,16 +6216,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:B12"/>
+  <dimension ref="A3:B48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="60.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="82.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -5949,74 +6238,362 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
-        <v>176</v>
+        <v>17</v>
       </c>
       <c r="B4" s="22">
-        <v>599</v>
+        <v>2748.99</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
-        <v>147</v>
+        <v>61</v>
       </c>
       <c r="B5" s="22">
-        <v>369</v>
+        <v>1719</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
-        <v>146</v>
+        <v>56</v>
       </c>
       <c r="B6" s="22">
-        <v>399</v>
+        <v>3559</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
-        <v>145</v>
+        <v>40</v>
       </c>
       <c r="B7" s="22">
-        <v>480</v>
+        <v>2029</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
-        <v>149</v>
+        <v>57</v>
       </c>
       <c r="B8" s="22">
-        <v>419</v>
+        <v>2409</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
-        <v>151</v>
+        <v>14</v>
       </c>
       <c r="B9" s="22">
-        <v>448.99</v>
+        <v>1719</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
-        <v>175</v>
+        <v>4</v>
       </c>
       <c r="B10" s="22">
-        <v>299</v>
+        <v>1368.99</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
-        <v>144</v>
+        <v>18</v>
       </c>
       <c r="B11" s="22">
-        <v>279</v>
+        <v>2058.9899999999998</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="22">
+        <v>908.99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="22">
+        <v>2179</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="22">
+        <v>1138.99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="22">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="22">
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="22">
+        <v>1259</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="22">
+        <v>2639</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="22">
+        <v>1828.99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="22">
+        <v>1489</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" s="22">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="22">
+        <v>448.99</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" s="22">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="22">
+        <v>6888.99</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" s="22">
+        <v>1489</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" s="22">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" s="22">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" s="22">
+        <v>1368.99</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" s="22">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" s="22">
+        <v>2179</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="B31" s="22">
+        <v>218.99</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B32" s="22">
+        <v>2179</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" s="22">
+        <v>3208.99</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34" s="22">
+        <v>1949</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B35" s="22">
+        <v>2058.9899999999998</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B36" s="22">
+        <v>1489</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37" s="22">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B38" s="22">
+        <v>1138.99</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B39" s="22">
+        <v>1419</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B40" s="22">
+        <v>1259</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B41" s="22">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B42" s="22">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B43" s="22">
+        <v>2639</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="B44" s="22">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="B45" s="22">
+        <v>1029</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B46" s="22">
+        <v>1138.99</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="B47" s="22">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="B12" s="22">
-        <v>3292.99</v>
+      <c r="B48" s="22">
+        <v>69265.86</v>
       </c>
     </row>
   </sheetData>
@@ -6035,10 +6612,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K143"/>
+  <dimension ref="A1:K152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="D85" sqref="D85"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="F70" sqref="F70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6068,10 +6645,10 @@
       <c r="E1" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="F1" s="43" t="s">
+      <c r="F1" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="G1" s="41" t="s">
         <v>1</v>
       </c>
       <c r="H1" s="14" t="s">
@@ -6100,13 +6677,13 @@
       <c r="D2" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="E2" s="41" t="s">
+      <c r="E2" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="F2" s="46" t="s">
+      <c r="F2" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="47">
+      <c r="G2" s="45">
         <v>2058.9899999999998</v>
       </c>
       <c r="H2" s="9">
@@ -6129,13 +6706,13 @@
       <c r="D3" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="40" t="s">
         <v>113</v>
       </c>
-      <c r="F3" s="48" t="s">
+      <c r="F3" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="49">
+      <c r="G3" s="47">
         <v>339</v>
       </c>
       <c r="H3" s="11">
@@ -6158,13 +6735,13 @@
       <c r="D4" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="E4" s="41" t="s">
+      <c r="E4" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="F4" s="46" t="s">
+      <c r="F4" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="47">
+      <c r="G4" s="45">
         <v>1368.99</v>
       </c>
       <c r="H4" s="9">
@@ -6187,13 +6764,13 @@
       <c r="D5" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="E5" s="42" t="s">
+      <c r="E5" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="F5" s="48" t="s">
+      <c r="F5" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="49">
+      <c r="G5" s="47">
         <v>1259</v>
       </c>
       <c r="H5" s="11">
@@ -6216,13 +6793,13 @@
       <c r="D6" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="E6" s="41" t="s">
+      <c r="E6" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="F6" s="46" t="s">
+      <c r="F6" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="47">
+      <c r="G6" s="45">
         <v>6888.99</v>
       </c>
       <c r="H6" s="9">
@@ -6245,13 +6822,13 @@
       <c r="D7" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="E7" s="42" t="s">
+      <c r="E7" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="F7" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7" s="49">
+      <c r="F7" s="46" t="s">
+        <v>268</v>
+      </c>
+      <c r="G7" s="47">
         <v>2639</v>
       </c>
       <c r="H7" s="11">
@@ -6274,13 +6851,13 @@
       <c r="D8" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="E8" s="41" t="s">
+      <c r="E8" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="F8" s="46" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" s="47">
+      <c r="F8" s="44" t="s">
+        <v>269</v>
+      </c>
+      <c r="G8" s="45">
         <v>1949</v>
       </c>
       <c r="H8" s="9">
@@ -6303,13 +6880,13 @@
       <c r="D9" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="E9" s="42" t="s">
+      <c r="E9" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="F9" s="48" t="s">
+      <c r="F9" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="49">
+      <c r="G9" s="47">
         <v>1368.99</v>
       </c>
       <c r="H9" s="11">
@@ -6332,13 +6909,13 @@
       <c r="D10" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="E10" s="41" t="s">
+      <c r="E10" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="F10" s="46" t="s">
+      <c r="F10" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="47">
+      <c r="G10" s="45">
         <v>1138.99</v>
       </c>
       <c r="H10" s="9">
@@ -6361,13 +6938,13 @@
       <c r="D11" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="E11" s="42" t="s">
+      <c r="E11" s="40" t="s">
         <v>113</v>
       </c>
-      <c r="F11" s="48" t="s">
+      <c r="F11" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="49">
+      <c r="G11" s="47">
         <v>739</v>
       </c>
       <c r="H11" s="11">
@@ -6390,13 +6967,13 @@
       <c r="D12" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="E12" s="41" t="s">
+      <c r="E12" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="F12" s="46" t="s">
+      <c r="F12" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="47">
+      <c r="G12" s="45">
         <v>2639</v>
       </c>
       <c r="H12" s="9">
@@ -6419,13 +6996,13 @@
       <c r="D13" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="E13" s="42" t="s">
+      <c r="E13" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="F13" s="48" t="s">
+      <c r="F13" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="G13" s="49">
+      <c r="G13" s="47">
         <v>3208.99</v>
       </c>
       <c r="H13" s="11">
@@ -6448,13 +7025,13 @@
       <c r="D14" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="E14" s="41" t="s">
+      <c r="E14" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="F14" s="46" t="s">
+      <c r="F14" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="G14" s="47">
+      <c r="G14" s="45">
         <v>1719</v>
       </c>
       <c r="H14" s="9">
@@ -6477,13 +7054,13 @@
       <c r="D15" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="E15" s="42" t="s">
+      <c r="E15" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="F15" s="48" t="s">
+      <c r="F15" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="G15" s="49">
+      <c r="G15" s="47">
         <v>2179</v>
       </c>
       <c r="H15" s="11">
@@ -6506,13 +7083,13 @@
       <c r="D16" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="E16" s="41" t="s">
+      <c r="E16" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="F16" s="46" t="s">
+      <c r="F16" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="G16" s="47">
+      <c r="G16" s="45">
         <v>1489</v>
       </c>
       <c r="H16" s="9">
@@ -6535,13 +7112,13 @@
       <c r="D17" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="E17" s="42" t="s">
+      <c r="E17" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="F17" s="48" t="s">
+      <c r="F17" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="G17" s="49">
+      <c r="G17" s="47">
         <v>2748.99</v>
       </c>
       <c r="H17" s="11">
@@ -6564,13 +7141,13 @@
       <c r="D18" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="E18" s="41" t="s">
+      <c r="E18" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="F18" s="46" t="s">
+      <c r="F18" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="G18" s="47">
+      <c r="G18" s="45">
         <v>2058.9899999999998</v>
       </c>
       <c r="H18" s="9">
@@ -6593,13 +7170,13 @@
       <c r="D19" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="E19" s="42" t="s">
+      <c r="E19" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="F19" s="48" t="s">
+      <c r="F19" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="G19" s="49">
+      <c r="G19" s="47">
         <v>1828.99</v>
       </c>
       <c r="H19" s="11">
@@ -6622,13 +7199,13 @@
       <c r="D20" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="E20" s="41" t="s">
+      <c r="E20" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="F20" s="46" t="s">
+      <c r="F20" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="G20" s="47">
+      <c r="G20" s="45">
         <v>1489</v>
       </c>
       <c r="H20" s="9">
@@ -6651,13 +7228,13 @@
       <c r="D21" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="E21" s="42" t="s">
+      <c r="E21" s="40" t="s">
         <v>113</v>
       </c>
-      <c r="F21" s="48" t="s">
+      <c r="F21" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="G21" s="49">
+      <c r="G21" s="47">
         <v>739</v>
       </c>
       <c r="H21" s="11">
@@ -6680,13 +7257,13 @@
       <c r="D22" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="E22" s="41" t="s">
+      <c r="E22" s="39" t="s">
         <v>113</v>
       </c>
-      <c r="F22" s="46" t="s">
+      <c r="F22" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="G22" s="47">
+      <c r="G22" s="45">
         <v>569</v>
       </c>
       <c r="H22" s="9">
@@ -6709,13 +7286,13 @@
       <c r="D23" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="E23" s="42" t="s">
+      <c r="E23" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="F23" s="48" t="s">
+      <c r="F23" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="G23" s="49">
+      <c r="G23" s="47">
         <v>1419</v>
       </c>
       <c r="H23" s="11">
@@ -6738,13 +7315,13 @@
       <c r="D24" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="E24" s="41" t="s">
+      <c r="E24" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="F24" s="46" t="s">
+      <c r="F24" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="G24" s="47">
+      <c r="G24" s="45">
         <v>2179</v>
       </c>
       <c r="H24" s="9">
@@ -6767,13 +7344,13 @@
       <c r="D25" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="E25" s="42" t="s">
+      <c r="E25" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="F25" s="48" t="s">
+      <c r="F25" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="G25" s="49">
+      <c r="G25" s="47">
         <v>908.99</v>
       </c>
       <c r="H25" s="11">
@@ -6796,13 +7373,13 @@
       <c r="D26" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="E26" s="41" t="s">
+      <c r="E26" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="F26" s="46" t="s">
+      <c r="F26" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="G26" s="47">
+      <c r="G26" s="45">
         <v>2179</v>
       </c>
       <c r="H26" s="9">
@@ -6825,13 +7402,13 @@
       <c r="D27" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="E27" s="42" t="s">
+      <c r="E27" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="F27" s="48" t="s">
+      <c r="F27" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="G27" s="49">
+      <c r="G27" s="47">
         <v>1138.99</v>
       </c>
       <c r="H27" s="11">
@@ -6854,13 +7431,13 @@
       <c r="D28" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="E28" s="41" t="s">
+      <c r="E28" s="39" t="s">
         <v>113</v>
       </c>
-      <c r="F28" s="46" t="s">
+      <c r="F28" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="G28" s="47">
+      <c r="G28" s="45">
         <v>629</v>
       </c>
       <c r="H28" s="9">
@@ -6883,13 +7460,13 @@
       <c r="D29" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="E29" s="42" t="s">
+      <c r="E29" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="F29" s="48" t="s">
+      <c r="F29" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="G29" s="49">
+      <c r="G29" s="47">
         <v>1089</v>
       </c>
       <c r="H29" s="11">
@@ -6912,13 +7489,13 @@
       <c r="D30" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="E30" s="41" t="s">
+      <c r="E30" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="F30" s="46" t="s">
+      <c r="F30" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="G30" s="47">
+      <c r="G30" s="45">
         <v>629</v>
       </c>
       <c r="H30" s="9">
@@ -6941,13 +7518,13 @@
       <c r="D31" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="E31" s="42" t="s">
+      <c r="E31" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="F31" s="48" t="s">
+      <c r="F31" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="G31" s="49">
+      <c r="G31" s="47">
         <v>629</v>
       </c>
       <c r="H31" s="11">
@@ -6970,13 +7547,13 @@
       <c r="D32" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="E32" s="41" t="s">
+      <c r="E32" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="F32" s="46" t="s">
+      <c r="F32" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="G32" s="47">
+      <c r="G32" s="45">
         <v>629</v>
       </c>
       <c r="H32" s="9">
@@ -6999,13 +7576,13 @@
       <c r="D33" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="E33" s="42" t="s">
+      <c r="E33" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="F33" s="48" t="s">
+      <c r="F33" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="G33" s="49">
+      <c r="G33" s="47">
         <v>629</v>
       </c>
       <c r="H33" s="11">
@@ -7028,13 +7605,13 @@
       <c r="D34" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="E34" s="41" t="s">
+      <c r="E34" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="F34" s="46" t="s">
+      <c r="F34" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="G34" s="47">
+      <c r="G34" s="45">
         <v>629</v>
       </c>
       <c r="H34" s="9">
@@ -7057,13 +7634,13 @@
       <c r="D35" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="E35" s="42" t="s">
+      <c r="E35" s="40" t="s">
         <v>113</v>
       </c>
-      <c r="F35" s="48" t="s">
+      <c r="F35" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="G35" s="49">
+      <c r="G35" s="47">
         <v>1029</v>
       </c>
       <c r="H35" s="11">
@@ -7086,13 +7663,13 @@
       <c r="D36" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="E36" s="41" t="s">
+      <c r="E36" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="F36" s="46" t="s">
+      <c r="F36" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="G36" s="47">
+      <c r="G36" s="45">
         <v>739</v>
       </c>
       <c r="H36" s="9">
@@ -7115,13 +7692,13 @@
       <c r="D37" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="E37" s="42" t="s">
+      <c r="E37" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="F37" s="48" t="s">
+      <c r="F37" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="G37" s="49">
+      <c r="G37" s="47">
         <v>1259</v>
       </c>
       <c r="H37" s="11">
@@ -7144,13 +7721,13 @@
       <c r="D38" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="E38" s="41" t="s">
+      <c r="E38" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="F38" s="46" t="s">
+      <c r="F38" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="G38" s="47">
+      <c r="G38" s="45">
         <v>1029</v>
       </c>
       <c r="H38" s="9">
@@ -7175,13 +7752,13 @@
       <c r="D39" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="E39" s="42" t="s">
+      <c r="E39" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="F39" s="48" t="s">
+      <c r="F39" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="G39" s="49">
+      <c r="G39" s="47">
         <v>629</v>
       </c>
       <c r="H39" s="11">
@@ -7204,13 +7781,13 @@
       <c r="D40" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="E40" s="41" t="s">
+      <c r="E40" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="F40" s="46" t="s">
+      <c r="F40" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="G40" s="47">
+      <c r="G40" s="45">
         <v>2029</v>
       </c>
       <c r="H40" s="9">
@@ -7233,13 +7810,13 @@
       <c r="D41" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="E41" s="42" t="s">
+      <c r="E41" s="40" t="s">
         <v>113</v>
       </c>
-      <c r="F41" s="48" t="s">
+      <c r="F41" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="G41" s="49">
+      <c r="G41" s="47">
         <v>739</v>
       </c>
       <c r="H41" s="11">
@@ -7262,13 +7839,13 @@
       <c r="D42" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="E42" s="41" t="s">
+      <c r="E42" s="39" t="s">
         <v>113</v>
       </c>
-      <c r="F42" s="46" t="s">
+      <c r="F42" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="G42" s="47">
+      <c r="G42" s="45">
         <v>908.99</v>
       </c>
       <c r="H42" s="9">
@@ -7291,13 +7868,13 @@
       <c r="D43" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="E43" s="42" t="s">
+      <c r="E43" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="F43" s="48" t="s">
+      <c r="F43" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="G43" s="49">
+      <c r="G43" s="47">
         <v>1138.99</v>
       </c>
       <c r="H43" s="11">
@@ -7320,13 +7897,13 @@
       <c r="D44" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="E44" s="41" t="s">
+      <c r="E44" s="39" t="s">
         <v>113</v>
       </c>
-      <c r="F44" s="46" t="s">
+      <c r="F44" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="G44" s="47">
+      <c r="G44" s="45">
         <v>279</v>
       </c>
       <c r="H44" s="9">
@@ -7349,13 +7926,13 @@
       <c r="D45" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="E45" s="42" t="s">
+      <c r="E45" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="F45" s="48" t="s">
+      <c r="F45" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="G45" s="49">
+      <c r="G45" s="47">
         <v>799</v>
       </c>
       <c r="H45" s="11">
@@ -7378,13 +7955,13 @@
       <c r="D46" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="E46" s="41" t="s">
+      <c r="E46" s="39" t="s">
         <v>113</v>
       </c>
-      <c r="F46" s="46" t="s">
+      <c r="F46" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="G46" s="47">
+      <c r="G46" s="45">
         <v>419</v>
       </c>
       <c r="H46" s="9">
@@ -7407,13 +7984,13 @@
       <c r="D47" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="E47" s="42" t="s">
+      <c r="E47" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="F47" s="48" t="s">
+      <c r="F47" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="G47" s="49">
+      <c r="G47" s="47">
         <v>509</v>
       </c>
       <c r="H47" s="11">
@@ -7436,13 +8013,13 @@
       <c r="D48" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="E48" s="41" t="s">
+      <c r="E48" s="39" t="s">
         <v>113</v>
       </c>
-      <c r="F48" s="46" t="s">
+      <c r="F48" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="G48" s="47">
+      <c r="G48" s="45">
         <v>339</v>
       </c>
       <c r="H48" s="9">
@@ -7465,13 +8042,13 @@
       <c r="D49" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="E49" s="42" t="s">
+      <c r="E49" s="40" t="s">
         <v>113</v>
       </c>
-      <c r="F49" s="48" t="s">
+      <c r="F49" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="G49" s="49">
+      <c r="G49" s="47">
         <v>339</v>
       </c>
       <c r="H49" s="11">
@@ -7494,13 +8071,13 @@
       <c r="D50" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="E50" s="41" t="s">
+      <c r="E50" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="F50" s="46" t="s">
+      <c r="F50" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="G50" s="47">
+      <c r="G50" s="45">
         <v>218.99</v>
       </c>
       <c r="H50" s="9">
@@ -7525,13 +8102,13 @@
       <c r="D51" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="E51" s="42" t="s">
+      <c r="E51" s="40" t="s">
         <v>113</v>
       </c>
-      <c r="F51" s="48" t="s">
+      <c r="F51" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="G51" s="49">
+      <c r="G51" s="47">
         <v>279</v>
       </c>
       <c r="H51" s="11">
@@ -7554,13 +8131,13 @@
       <c r="D52" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="E52" s="41" t="s">
+      <c r="E52" s="39" t="s">
         <v>113</v>
       </c>
-      <c r="F52" s="46" t="s">
+      <c r="F52" s="44" t="s">
         <v>52</v>
       </c>
-      <c r="G52" s="47">
+      <c r="G52" s="45">
         <v>479</v>
       </c>
       <c r="H52" s="9">
@@ -7585,13 +8162,13 @@
       <c r="D53" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="E53" s="42" t="s">
+      <c r="E53" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="F53" s="48" t="s">
+      <c r="F53" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="G53" s="49">
+      <c r="G53" s="47">
         <v>448.99</v>
       </c>
       <c r="H53" s="11">
@@ -7614,13 +8191,13 @@
       <c r="D54" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="E54" s="41" t="s">
+      <c r="E54" s="39" t="s">
         <v>113</v>
       </c>
-      <c r="F54" s="46" t="s">
+      <c r="F54" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="G54" s="47">
+      <c r="G54" s="45">
         <v>339</v>
       </c>
       <c r="H54" s="9">
@@ -7645,13 +8222,13 @@
       <c r="D55" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="E55" s="42" t="s">
+      <c r="E55" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="F55" s="48" t="s">
+      <c r="F55" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="G55" s="49">
+      <c r="G55" s="47">
         <v>1489</v>
       </c>
       <c r="H55" s="11">
@@ -7674,13 +8251,13 @@
       <c r="D56" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="E56" s="41" t="s">
+      <c r="E56" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="F56" s="46" t="s">
+      <c r="F56" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="G56" s="47">
+      <c r="G56" s="45">
         <v>3559</v>
       </c>
       <c r="H56" s="9">
@@ -7703,13 +8280,13 @@
       <c r="D57" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="E57" s="42" t="s">
+      <c r="E57" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="F57" s="48" t="s">
+      <c r="F57" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="G57" s="49">
+      <c r="G57" s="47">
         <v>2409</v>
       </c>
       <c r="H57" s="11">
@@ -7732,13 +8309,13 @@
       <c r="D58" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="E58" s="41" t="s">
+      <c r="E58" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="F58" s="46" t="s">
+      <c r="F58" s="44" t="s">
         <v>58</v>
       </c>
-      <c r="G58" s="47">
+      <c r="G58" s="45">
         <v>569</v>
       </c>
       <c r="H58" s="9">
@@ -7761,13 +8338,13 @@
       <c r="D59" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="E59" s="42" t="s">
+      <c r="E59" s="40" t="s">
         <v>113</v>
       </c>
-      <c r="F59" s="48" t="s">
+      <c r="F59" s="46" t="s">
         <v>59</v>
       </c>
-      <c r="G59" s="49">
+      <c r="G59" s="47">
         <v>1489</v>
       </c>
       <c r="H59" s="11">
@@ -7790,13 +8367,13 @@
       <c r="D60" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="E60" s="41" t="s">
+      <c r="E60" s="39" t="s">
         <v>113</v>
       </c>
-      <c r="F60" s="46" t="s">
+      <c r="F60" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="G60" s="47">
+      <c r="G60" s="45">
         <v>799</v>
       </c>
       <c r="H60" s="9">
@@ -7821,13 +8398,13 @@
       <c r="D61" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="E61" s="42" t="s">
+      <c r="E61" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="F61" s="48" t="s">
+      <c r="F61" s="46" t="s">
         <v>61</v>
       </c>
-      <c r="G61" s="49">
+      <c r="G61" s="47">
         <v>1719</v>
       </c>
       <c r="H61" s="11">
@@ -7850,13 +8427,13 @@
       <c r="D62" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="E62" s="41" t="s">
+      <c r="E62" s="39" t="s">
         <v>113</v>
       </c>
-      <c r="F62" s="46" t="s">
+      <c r="F62" s="44" t="s">
         <v>62</v>
       </c>
-      <c r="G62" s="47">
+      <c r="G62" s="45">
         <v>999.01</v>
       </c>
       <c r="H62" s="9">
@@ -7879,13 +8456,13 @@
       <c r="D63" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="E63" s="42" t="s">
+      <c r="E63" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="F63" s="48" t="s">
+      <c r="F63" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="G63" s="49">
+      <c r="G63" s="47">
         <v>629</v>
       </c>
       <c r="H63" s="11">
@@ -7911,10 +8488,10 @@
       <c r="E64" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="F64" s="44" t="s">
+      <c r="F64" s="42" t="s">
         <v>124</v>
       </c>
-      <c r="G64" s="45">
+      <c r="G64" s="43">
         <v>1099</v>
       </c>
       <c r="H64" s="10">
@@ -10105,13 +10682,13 @@
       <c r="K139" s="27"/>
     </row>
     <row r="140" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A140" s="36" t="s">
+      <c r="A140" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="B140" s="36" t="s">
+      <c r="B140" s="34" t="s">
         <v>251</v>
       </c>
-      <c r="C140" s="32" t="s">
+      <c r="C140" s="30" t="s">
         <v>90</v>
       </c>
       <c r="D140" s="19" t="s">
@@ -10120,27 +10697,27 @@
       <c r="E140" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="F140" s="37" t="s">
+      <c r="F140" s="35" t="s">
         <v>253</v>
       </c>
-      <c r="G140" s="38">
+      <c r="G140" s="36">
         <v>1000</v>
       </c>
-      <c r="H140" s="37">
+      <c r="H140" s="35">
         <v>4</v>
       </c>
-      <c r="I140" s="39"/>
-      <c r="J140" s="40"/>
-      <c r="K140" s="40"/>
+      <c r="I140" s="37"/>
+      <c r="J140" s="38"/>
+      <c r="K140" s="38"/>
     </row>
     <row r="141" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A141" s="36" t="s">
+      <c r="A141" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="B141" s="36" t="s">
+      <c r="B141" s="34" t="s">
         <v>251</v>
       </c>
-      <c r="C141" s="37" t="s">
+      <c r="C141" s="35" t="s">
         <v>252</v>
       </c>
       <c r="D141" s="19" t="s">
@@ -10149,76 +10726,337 @@
       <c r="E141" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="F141" s="37" t="s">
+      <c r="F141" s="35" t="s">
         <v>254</v>
       </c>
-      <c r="G141" s="38">
+      <c r="G141" s="36">
         <v>1159</v>
       </c>
-      <c r="H141" s="37">
+      <c r="H141" s="35">
         <v>4</v>
       </c>
-      <c r="I141" s="39"/>
-      <c r="J141" s="40"/>
-      <c r="K141" s="40"/>
+      <c r="I141" s="37"/>
+      <c r="J141" s="38"/>
+      <c r="K141" s="38"/>
     </row>
     <row r="142" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A142" s="31" t="s">
+      <c r="A142" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="B142" s="31" t="s">
+      <c r="B142" s="29" t="s">
         <v>251</v>
       </c>
       <c r="C142" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="D142" s="32" t="s">
+      <c r="D142" s="30" t="s">
         <v>73</v>
       </c>
       <c r="E142" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="F142" s="37" t="s">
+      <c r="F142" s="35" t="s">
         <v>255</v>
       </c>
-      <c r="G142" s="33">
+      <c r="G142" s="31">
         <v>1280</v>
       </c>
-      <c r="H142" s="32">
+      <c r="H142" s="30">
         <v>4</v>
       </c>
-      <c r="I142" s="34"/>
-      <c r="J142" s="35"/>
-      <c r="K142" s="35"/>
+      <c r="I142" s="32"/>
+      <c r="J142" s="33"/>
+      <c r="K142" s="33"/>
     </row>
     <row r="143" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A143" s="36" t="s">
+      <c r="A143" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="B143" s="36" t="s">
+      <c r="B143" s="34" t="s">
         <v>251</v>
       </c>
       <c r="C143" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="D143" s="37" t="s">
+      <c r="D143" s="35" t="s">
         <v>73</v>
       </c>
       <c r="E143" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="F143" s="37" t="s">
+      <c r="F143" s="35" t="s">
         <v>256</v>
       </c>
-      <c r="G143" s="38">
+      <c r="G143" s="36">
         <v>1199</v>
       </c>
-      <c r="H143" s="37">
+      <c r="H143" s="35">
         <v>4</v>
       </c>
-      <c r="I143" s="39"/>
-      <c r="J143" s="40"/>
-      <c r="K143" s="40"/>
+      <c r="I143" s="37"/>
+      <c r="J143" s="38"/>
+      <c r="K143" s="38"/>
+    </row>
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A144" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="B144" s="18" t="s">
+        <v>214</v>
+      </c>
+      <c r="C144" s="35" t="s">
+        <v>252</v>
+      </c>
+      <c r="D144" s="19" t="s">
+        <v>239</v>
+      </c>
+      <c r="E144" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="F144" s="50" t="s">
+        <v>257</v>
+      </c>
+      <c r="G144" s="20">
+        <v>445</v>
+      </c>
+      <c r="H144" s="19">
+        <v>4</v>
+      </c>
+      <c r="I144" s="25"/>
+      <c r="J144" s="27"/>
+      <c r="K144" s="27"/>
+    </row>
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A145" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="B145" s="18" t="s">
+        <v>214</v>
+      </c>
+      <c r="C145" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D145" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="E145" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="F145" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="G145" s="20">
+        <v>699</v>
+      </c>
+      <c r="H145" s="19">
+        <v>4</v>
+      </c>
+      <c r="I145" s="25"/>
+      <c r="J145" s="27"/>
+      <c r="K145" s="27"/>
+    </row>
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A146" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="B146" s="18" t="s">
+        <v>214</v>
+      </c>
+      <c r="C146" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D146" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="E146" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="F146" s="19" t="s">
+        <v>259</v>
+      </c>
+      <c r="G146" s="20">
+        <v>180</v>
+      </c>
+      <c r="H146" s="19">
+        <v>5</v>
+      </c>
+      <c r="I146" s="25"/>
+      <c r="J146" s="27"/>
+      <c r="K146" s="27"/>
+    </row>
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A147" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="B147" s="18" t="s">
+        <v>214</v>
+      </c>
+      <c r="C147" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="D147" s="19" t="s">
+        <v>261</v>
+      </c>
+      <c r="E147" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="F147" s="19" t="s">
+        <v>260</v>
+      </c>
+      <c r="G147" s="20">
+        <v>180</v>
+      </c>
+      <c r="H147" s="19">
+        <v>3.5</v>
+      </c>
+      <c r="I147" s="25"/>
+      <c r="J147" s="27"/>
+      <c r="K147" s="27"/>
+    </row>
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A148" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="B148" s="18" t="s">
+        <v>214</v>
+      </c>
+      <c r="C148" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="D148" s="19" t="s">
+        <v>263</v>
+      </c>
+      <c r="E148" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="F148" s="19" t="s">
+        <v>262</v>
+      </c>
+      <c r="G148" s="20">
+        <v>180</v>
+      </c>
+      <c r="H148" s="19">
+        <v>3.5</v>
+      </c>
+      <c r="I148" s="25"/>
+      <c r="J148" s="27"/>
+      <c r="K148" s="27"/>
+    </row>
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A149" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="B149" s="18" t="s">
+        <v>214</v>
+      </c>
+      <c r="C149" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D149" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="E149" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="F149" s="19" t="s">
+        <v>264</v>
+      </c>
+      <c r="G149" s="20">
+        <v>699</v>
+      </c>
+      <c r="H149" s="19">
+        <v>5</v>
+      </c>
+      <c r="I149" s="25"/>
+      <c r="J149" s="27"/>
+      <c r="K149" s="27"/>
+    </row>
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A150" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="B150" s="18" t="s">
+        <v>215</v>
+      </c>
+      <c r="C150" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="D150" s="19" t="s">
+        <v>239</v>
+      </c>
+      <c r="E150" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="F150" s="19" t="s">
+        <v>265</v>
+      </c>
+      <c r="G150" s="20">
+        <v>413</v>
+      </c>
+      <c r="H150" s="19">
+        <v>4</v>
+      </c>
+      <c r="I150" s="25"/>
+      <c r="J150" s="27"/>
+      <c r="K150" s="27"/>
+    </row>
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A151" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B151" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="C151" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D151" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="E151" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="F151" s="12" t="s">
+        <v>267</v>
+      </c>
+      <c r="G151" s="17">
+        <v>320</v>
+      </c>
+      <c r="H151" s="12">
+        <v>4</v>
+      </c>
+      <c r="I151" s="25"/>
+      <c r="J151" s="27"/>
+      <c r="K151" s="27"/>
+    </row>
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A152" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="B152" s="18" t="s">
+        <v>216</v>
+      </c>
+      <c r="C152" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D152" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="E152" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="F152" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="G152" s="20">
+        <v>345</v>
+      </c>
+      <c r="H152" s="19">
+        <v>4</v>
+      </c>
+      <c r="I152" s="25"/>
+      <c r="J152" s="27"/>
+      <c r="K152" s="27"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -10226,8 +11064,9 @@
     <hyperlink ref="F130" r:id="rId2" display="https://www.ttartisan.com/?AF-Lens/AF-35-II.html"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>